<commit_message>
For reals updated GDP
</commit_message>
<xml_diff>
--- a/gdp_data.xlsx
+++ b/gdp_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mila/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE97FDA5-0CFE-D744-8B8C-BB3D09503CCE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66634FF4-58BF-1344-A3A5-021F1EE373D4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -878,7 +878,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -930,7 +930,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1134,7 +1134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>

</xml_diff>